<commit_message>
Add flowthrough data to separate dataframe and update output file
</commit_message>
<xml_diff>
--- a/TN037/TN037.3_output.xlsx
+++ b/TN037/TN037.3_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -833,6 +833,348 @@
         <v>0.590495589788456</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>-23.511945</v>
+      </c>
+      <c r="E20" t="n">
+        <v>8.359865661106497e-06</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>-21.839316</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2.665083369387191e-05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>-22.082388</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2.251846775642507e-05</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>-9.168227000000002</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.1738155655915517</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>-8.392045999999997</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2976750457239626</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>-8.591697</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.2592038747363474</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>-4.581559000000002</v>
+      </c>
+      <c r="E26" t="n">
+        <v>4.176507966076688</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>-5.376252000000001</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2.407614131490228</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>flowthrough1</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>-5.448609999999999</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2.289839039155415</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>flowthrough1_no_beads</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Calculate flowthrough and enrich individually and graph separately
</commit_message>
<xml_diff>
--- a/TN037/TN037.3_output.xlsx
+++ b/TN037/TN037.3_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,7 +839,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -848,10 +848,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>-23.511945</v>
+        <v>-0.3637975000000004</v>
       </c>
       <c r="E20" t="n">
-        <v>8.359865661106497e-06</v>
+        <v>77.71163389690619</v>
       </c>
     </row>
     <row r="21">
@@ -860,7 +860,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -869,10 +869,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>-21.839316</v>
+        <v>-0.8250100000000007</v>
       </c>
       <c r="E21" t="n">
-        <v>2.665083369387191e-05</v>
+        <v>56.44782897241549</v>
       </c>
     </row>
     <row r="22">
@@ -881,7 +881,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -890,10 +890,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>-22.082388</v>
+        <v>-0.2946559999999998</v>
       </c>
       <c r="E22" t="n">
-        <v>2.251846775642507e-05</v>
+        <v>81.52667035655602</v>
       </c>
     </row>
     <row r="23">
@@ -902,7 +902,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -911,10 +911,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>-9.168227000000002</v>
+        <v>-0.05201100000000025</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1738155655915517</v>
+        <v>96.45908299185442</v>
       </c>
     </row>
     <row r="24">
@@ -923,7 +923,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -932,10 +932,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>-8.392045999999997</v>
+        <v>-0.5995480000000022</v>
       </c>
       <c r="E24" t="n">
-        <v>0.2976750457239626</v>
+        <v>65.9960690350554</v>
       </c>
     </row>
     <row r="25">
@@ -944,7 +944,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -953,10 +953,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>-8.591697</v>
+        <v>-0.4344429999999981</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2592038747363474</v>
+        <v>73.99793929296716</v>
       </c>
     </row>
     <row r="26">
@@ -965,7 +965,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -974,10 +974,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>-4.581559000000002</v>
+        <v>-2.535222999999998</v>
       </c>
       <c r="E26" t="n">
-        <v>4.176507966076688</v>
+        <v>17.25130014647654</v>
       </c>
     </row>
     <row r="27">
@@ -986,7 +986,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -995,10 +995,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>-5.376252000000001</v>
+        <v>-2.086707999999998</v>
       </c>
       <c r="E27" t="n">
-        <v>2.407614131490228</v>
+        <v>23.54172595260836</v>
       </c>
     </row>
     <row r="28">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>flowthrough1</t>
+          <t>flowthrough1_beads</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1016,15 +1016,15 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>-5.448609999999999</v>
+        <v>-2.067386000000003</v>
       </c>
       <c r="E28" t="n">
-        <v>2.289839039155415</v>
+        <v>23.85914087148842</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1036,12 +1036,16 @@
           <t>RNA18S1</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>-0.5757679999999983</v>
+      </c>
+      <c r="E29" t="n">
+        <v>67.09289959562386</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1053,12 +1057,16 @@
           <t>RNA18S1</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>-0.7790359999999996</v>
+      </c>
+      <c r="E30" t="n">
+        <v>58.27560571999989</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1070,12 +1078,16 @@
           <t>RNA18S1</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>-1.10886</v>
+      </c>
+      <c r="E31" t="n">
+        <v>46.36602649074357</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1087,12 +1099,16 @@
           <t>vtRNA1-1</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+      <c r="D32" t="n">
+        <v>-0.243466999999999</v>
+      </c>
+      <c r="E32" t="n">
+        <v>84.4712906809921</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1104,12 +1120,16 @@
           <t>vtRNA1-1</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
+      <c r="D33" t="n">
+        <v>-0.4644119999999994</v>
+      </c>
+      <c r="E33" t="n">
+        <v>72.47664105276699</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1121,12 +1141,16 @@
           <t>vtRNA1-1</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>-0.07104799999999756</v>
+      </c>
+      <c r="E34" t="n">
+        <v>95.19462357058747</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1138,12 +1162,16 @@
           <t>FFLUC</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>-0.8912699999999987</v>
+      </c>
+      <c r="E35" t="n">
+        <v>53.91393066245682</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1155,12 +1183,16 @@
           <t>FFLUC</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>-1.017118</v>
+      </c>
+      <c r="E36" t="n">
+        <v>49.41024107858238</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1172,8 +1204,201 @@
           <t>FFLUC</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>-0.6482320000000001</v>
+      </c>
+      <c r="E37" t="n">
+        <v>63.80617693577092</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>-23.8757425</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6.496588196832256e-06</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>-22.664326</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1.504381702323968e-05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>RNA18S1</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>-22.377044</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.835855697712803e-05</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>-9.220238000000002</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.167660900666716</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>-8.991593999999999</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.1964538286761191</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>vtRNA1-1</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>-9.026139999999998</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.1918055258724211</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>-7.116782000000001</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.720501924869392</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>-7.462959999999999</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.5667939208317014</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>flowthrough2</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>FFLUC</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>-7.515996000000001</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.5463359220824272</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>